<commit_message>
Update for all split videos
</commit_message>
<xml_diff>
--- a/SodiumDisposal/Dataset/DatasetAnalysisReport.xlsx
+++ b/SodiumDisposal/Dataset/DatasetAnalysisReport.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="4"/>
@@ -16,12 +16,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Video Analysis'!$A$1:$M$76</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="341">
   <si>
     <t>AXIS 213 - 10.1.5.173 2024-07-04_11_51_08_772</t>
   </si>
@@ -768,13 +768,289 @@
   </si>
   <si>
     <t>14;18</t>
+  </si>
+  <si>
+    <t>2,23</t>
+  </si>
+  <si>
+    <t>5,29</t>
+  </si>
+  <si>
+    <t>29,79,101</t>
+  </si>
+  <si>
+    <t>20,33.73,87</t>
+  </si>
+  <si>
+    <t>26,35,76,89</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>3,15,30,39,70</t>
+  </si>
+  <si>
+    <t>5,25,34,46,79</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>8,31,36,51</t>
+  </si>
+  <si>
+    <t>13,34,51,55</t>
+  </si>
+  <si>
+    <t>25,41,53,59</t>
+  </si>
+  <si>
+    <t>30,50,59,62</t>
+  </si>
+  <si>
+    <t>39,58</t>
+  </si>
+  <si>
+    <t>51,61</t>
+  </si>
+  <si>
+    <t>27,36,57,70</t>
+  </si>
+  <si>
+    <t>31,44,64,77</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>67,80</t>
+  </si>
+  <si>
+    <t>73,84</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>34,92</t>
+  </si>
+  <si>
+    <t>25,44,67</t>
+  </si>
+  <si>
+    <t>33,47,73</t>
+  </si>
+  <si>
+    <t>4,38,55,59</t>
+  </si>
+  <si>
+    <t>13,41,59,62</t>
+  </si>
+  <si>
+    <t>16,22,46</t>
+  </si>
+  <si>
+    <t>19,25,49</t>
+  </si>
+  <si>
+    <t>42,50,55</t>
+  </si>
+  <si>
+    <t>48,52,58</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>25,29,69</t>
+  </si>
+  <si>
+    <t>27,36,73</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>20,24,29,44,55,58,74,82,97,107,124</t>
+  </si>
+  <si>
+    <t>37, 103</t>
+  </si>
+  <si>
+    <t>23, 27, 35, 49, 57, 63, 79, 92, 103, 113, 131</t>
+  </si>
+  <si>
+    <t>35, 84, 107</t>
+  </si>
+  <si>
+    <t>19,64,78</t>
+  </si>
+  <si>
+    <t>25,71,78</t>
+  </si>
+  <si>
+    <t>2,13,28,37,51,82,110,127,139,157, 181,196,247,271,286,310,321,329, 341,352,406,438,506,532,558,606,684,706,1093,1116,1134,1407,1429, 1443,1623,1656,1665,1725,1737, 1752, 1763,1769,1773,1953,2335,2476, 2485,2500,2545,2580</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>14,45,114,125,143,158,170,188,196, 279,332,361,389,427,451,524,596,608,626,646,680,703</t>
+  </si>
+  <si>
+    <t>27,55,124,130,150,166,184,190,277,321, 340,387,412,441,482,527,603,615,633,658, 690,713</t>
+  </si>
+  <si>
+    <t>45,73,114,130,151,169,175,221,262,277,309, 329,339,365,376,395,421,431,453,465,475,523, 543,574,589,601,609,624,643,673,679,711,717</t>
+  </si>
+  <si>
+    <t>5,20,32,41,56,92,114,131,152,167,189,207,251, 279,305,320,327,338,350,400,412,444,511,541, 569,610,689,712,1099,1120,1138,1410,1436, 1448,1626,1660,1668,1728,1750,1761,1767, 1773,1783,1958,2340,2483,2487,2504,2552,2603</t>
+  </si>
+  <si>
+    <t>36,48,76,126,131,153,172,180,237, 264,292,311,333,343,373,384,412,427,441, 462,472,478,526,546,578, 591,603,611,631,657,674,705,712</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>25,41,61,110,155</t>
+  </si>
+  <si>
+    <t>37,55,70,120,172</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>23,29,39</t>
+  </si>
+  <si>
+    <t>28,36,53</t>
+  </si>
+  <si>
+    <t>2,17,31</t>
+  </si>
+  <si>
+    <t>14,27,39</t>
+  </si>
+  <si>
+    <t>3,13,34,67</t>
+  </si>
+  <si>
+    <t>10,32,46,74</t>
+  </si>
+  <si>
+    <t>3,37,63,71,84</t>
+  </si>
+  <si>
+    <t>16,44,70,80,90</t>
+  </si>
+  <si>
+    <t>3,25,57</t>
+  </si>
+  <si>
+    <t>24,41,68</t>
+  </si>
+  <si>
+    <t>29,82</t>
+  </si>
+  <si>
+    <t>48,91</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>20,32</t>
+  </si>
+  <si>
+    <t>31,41</t>
+  </si>
+  <si>
+    <t>2,18,30</t>
+  </si>
+  <si>
+    <t>17,26,63</t>
+  </si>
+  <si>
+    <t>21,54</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>14,34,62</t>
+  </si>
+  <si>
+    <t>33,49,71</t>
+  </si>
+  <si>
+    <t>10,22</t>
+  </si>
+  <si>
+    <t>15,53</t>
+  </si>
+  <si>
+    <t>14,40</t>
+  </si>
+  <si>
+    <t>27,53</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -820,7 +1096,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1052,22 +1328,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1171,11 +1436,30 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1237,7 +1521,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1269,10 +1553,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1304,7 +1587,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1480,20 +1762,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1504,17 +1786,17 @@
         <v>9.0277777777777776E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="C3" s="2">
         <v>9.8611111111111108E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="C4" s="2">
         <v>0.10902777777777778</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="C5" s="2">
         <v>0.15486111111111112</v>
       </c>
@@ -1522,17 +1804,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="C6" s="2">
         <v>0.16180555555555556</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="C8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1543,12 +1825,12 @@
         <v>0.15555555555555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="C10" s="2">
         <v>0.16180555555555556</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1562,7 +1844,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1573,12 +1855,12 @@
         <v>0.21736111111111112</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="C13" s="2">
         <v>0.23124999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="C14" s="2">
         <v>0.27986111111111112</v>
       </c>
@@ -1589,14 +1871,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
@@ -1604,7 +1886,7 @@
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1618,7 +1900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -1629,7 +1911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1643,7 +1925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -1651,7 +1933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="C5" t="s">
         <v>14</v>
       </c>
@@ -1659,7 +1941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="C6" t="s">
         <v>16</v>
       </c>
@@ -1667,7 +1949,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -1678,7 +1960,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -1689,7 +1971,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1703,7 +1985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1717,7 +1999,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="C11" t="s">
         <v>33</v>
       </c>
@@ -1732,14 +2014,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="10"/>
     <col min="2" max="2" width="24" style="10" bestFit="1" customWidth="1"/>
@@ -1752,8 +2034,8 @@
     <col min="9" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" ht="20.25" thickBot="1"/>
+    <row r="2" spans="2:8" ht="20.25" thickBot="1">
       <c r="B2" s="15" t="s">
         <v>66</v>
       </c>
@@ -1776,7 +2058,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8">
       <c r="B3" s="31" t="s">
         <v>59</v>
       </c>
@@ -1799,7 +2081,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8">
       <c r="B4" s="14" t="s">
         <v>60</v>
       </c>
@@ -1822,7 +2104,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8">
       <c r="B5" s="14" t="s">
         <v>61</v>
       </c>
@@ -1845,7 +2127,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8">
       <c r="B6" s="14" t="s">
         <v>62</v>
       </c>
@@ -1868,7 +2150,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="20.25" thickBot="1">
       <c r="B7" s="32" t="s">
         <v>63</v>
       </c>
@@ -1897,7 +2179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1905,7 +2187,7 @@
       <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" style="6" bestFit="1" customWidth="1"/>
@@ -1920,7 +2202,7 @@
     <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
@@ -1961,7 +2243,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -1990,7 +2272,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
@@ -2022,7 +2304,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2057,7 +2339,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
@@ -2089,7 +2371,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
@@ -2119,7 +2401,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
@@ -2148,7 +2430,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="9" t="s">
         <v>2</v>
       </c>
@@ -2180,7 +2462,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
@@ -2209,7 +2491,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -2238,7 +2520,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
@@ -2267,7 +2549,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="9" t="s">
         <v>2</v>
       </c>
@@ -2299,7 +2581,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="9" t="s">
         <v>2</v>
       </c>
@@ -2328,7 +2610,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="9" t="s">
         <v>2</v>
       </c>
@@ -2360,7 +2642,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="9" t="s">
         <v>2</v>
       </c>
@@ -2392,7 +2674,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="9" t="s">
         <v>2</v>
       </c>
@@ -2424,7 +2706,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" s="9" t="s">
         <v>2</v>
       </c>
@@ -2453,7 +2735,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="9" t="s">
         <v>2</v>
       </c>
@@ -2482,7 +2764,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" s="9" t="s">
         <v>2</v>
       </c>
@@ -2511,7 +2793,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" s="9" t="s">
         <v>2</v>
       </c>
@@ -2540,7 +2822,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="9" t="s">
         <v>2</v>
       </c>
@@ -2569,7 +2851,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" s="9" t="s">
         <v>2</v>
       </c>
@@ -2598,7 +2880,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" s="9" t="s">
         <v>2</v>
       </c>
@@ -2627,7 +2909,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" s="9" t="s">
         <v>10</v>
       </c>
@@ -2656,7 +2938,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" s="9" t="s">
         <v>10</v>
       </c>
@@ -2685,7 +2967,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" s="9" t="s">
         <v>10</v>
       </c>
@@ -2717,7 +2999,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" s="9" t="s">
         <v>10</v>
       </c>
@@ -2746,7 +3028,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" s="9" t="s">
         <v>10</v>
       </c>
@@ -2775,7 +3057,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" s="9" t="s">
         <v>10</v>
       </c>
@@ -2804,7 +3086,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" s="9" t="s">
         <v>10</v>
       </c>
@@ -2833,7 +3115,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" s="9" t="s">
         <v>10</v>
       </c>
@@ -2865,7 +3147,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" s="9" t="s">
         <v>10</v>
       </c>
@@ -2894,7 +3176,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19">
       <c r="A33" s="9" t="s">
         <v>10</v>
       </c>
@@ -2923,7 +3205,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19">
       <c r="A34" s="9" t="s">
         <v>10</v>
       </c>
@@ -2959,7 +3241,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19">
       <c r="A35" s="9" t="s">
         <v>10</v>
       </c>
@@ -2988,7 +3270,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19">
       <c r="A36" s="9" t="s">
         <v>26</v>
       </c>
@@ -3020,7 +3302,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19">
       <c r="A37" s="9" t="s">
         <v>26</v>
       </c>
@@ -3055,7 +3337,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19">
       <c r="A38" s="9" t="s">
         <v>26</v>
       </c>
@@ -3084,7 +3366,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19">
       <c r="A39" s="9" t="s">
         <v>26</v>
       </c>
@@ -3113,7 +3395,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -3158,7 +3440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19">
       <c r="A41" s="9" t="s">
         <v>26</v>
       </c>
@@ -3187,7 +3469,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19">
       <c r="A42" s="9" t="s">
         <v>30</v>
       </c>
@@ -3219,7 +3501,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19">
       <c r="A43" s="9" t="s">
         <v>30</v>
       </c>
@@ -3251,7 +3533,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19">
       <c r="A44" s="9" t="s">
         <v>30</v>
       </c>
@@ -3283,7 +3565,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19">
       <c r="A45" s="9" t="s">
         <v>30</v>
       </c>
@@ -3315,7 +3597,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19">
       <c r="A46" s="9" t="s">
         <v>30</v>
       </c>
@@ -3344,7 +3626,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19">
       <c r="A47" s="9" t="s">
         <v>30</v>
       </c>
@@ -3373,7 +3655,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19">
       <c r="A48" s="9" t="s">
         <v>30</v>
       </c>
@@ -3402,7 +3684,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" s="9" t="s">
         <v>30</v>
       </c>
@@ -3431,7 +3713,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" s="9" t="s">
         <v>30</v>
       </c>
@@ -3466,7 +3748,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" s="9" t="s">
         <v>30</v>
       </c>
@@ -3498,7 +3780,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52" s="9" t="s">
         <v>30</v>
       </c>
@@ -3527,7 +3809,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53" s="9" t="s">
         <v>30</v>
       </c>
@@ -3556,7 +3838,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54" s="9" t="s">
         <v>30</v>
       </c>
@@ -3585,7 +3867,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55" s="9" t="s">
         <v>30</v>
       </c>
@@ -3620,7 +3902,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" s="9" t="s">
         <v>30</v>
       </c>
@@ -3652,7 +3934,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" s="9" t="s">
         <v>30</v>
       </c>
@@ -3681,7 +3963,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" s="9" t="s">
         <v>30</v>
       </c>
@@ -3710,7 +3992,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" s="9" t="s">
         <v>30</v>
       </c>
@@ -3742,7 +4024,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13">
       <c r="A60" s="9" t="s">
         <v>30</v>
       </c>
@@ -3774,7 +4056,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" s="9" t="s">
         <v>30</v>
       </c>
@@ -3803,7 +4085,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13">
       <c r="A62" s="9" t="s">
         <v>30</v>
       </c>
@@ -3832,7 +4114,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13">
       <c r="A63" s="9" t="s">
         <v>30</v>
       </c>
@@ -3864,7 +4146,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13">
       <c r="A64" s="9" t="s">
         <v>30</v>
       </c>
@@ -3899,7 +4181,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13">
       <c r="A65" s="9" t="s">
         <v>30</v>
       </c>
@@ -3934,7 +4216,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="A66" s="9" t="s">
         <v>30</v>
       </c>
@@ -3963,7 +4245,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13">
       <c r="A67" s="9" t="s">
         <v>30</v>
       </c>
@@ -3992,7 +4274,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13">
       <c r="A68" s="9" t="s">
         <v>30</v>
       </c>
@@ -4024,7 +4306,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13">
       <c r="A69" s="9" t="s">
         <v>30</v>
       </c>
@@ -4053,7 +4335,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13">
       <c r="A70" s="9" t="s">
         <v>30</v>
       </c>
@@ -4088,7 +4370,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13">
       <c r="A71" s="9" t="s">
         <v>30</v>
       </c>
@@ -4123,7 +4405,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="A72" s="9" t="s">
         <v>30</v>
       </c>
@@ -4152,7 +4434,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13">
       <c r="A73" s="9" t="s">
         <v>30</v>
       </c>
@@ -4187,7 +4469,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="A74" s="9" t="s">
         <v>30</v>
       </c>
@@ -4216,7 +4498,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" s="9" t="s">
         <v>30</v>
       </c>
@@ -4251,7 +4533,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13">
       <c r="A76" s="9" t="s">
         <v>30</v>
       </c>
@@ -4288,14 +4570,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="C70" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
@@ -4303,15 +4585,15 @@
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="36"/>
     <col min="7" max="7" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37" style="36" customWidth="1"/>
+    <col min="9" max="9" width="41.28515625" style="36" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="4" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
@@ -4336,7 +4618,7 @@
       <c r="H1" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="34" t="s">
         <v>100</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -4361,7 +4643,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="9" t="s">
         <v>30</v>
       </c>
@@ -4386,14 +4668,14 @@
       <c r="H2" s="36">
         <v>74</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="36">
         <v>77</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="9" t="s">
         <v>30</v>
       </c>
@@ -4412,11 +4694,11 @@
       <c r="F3" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
@@ -4435,11 +4717,11 @@
       <c r="F4" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
@@ -4464,14 +4746,14 @@
       <c r="H5" s="36">
         <v>31</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="36">
         <v>48</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="9" t="s">
         <v>30</v>
       </c>
@@ -4496,14 +4778,14 @@
       <c r="H6" s="36">
         <v>30</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="36">
         <v>40</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="9" t="s">
         <v>30</v>
       </c>
@@ -4528,14 +4810,14 @@
       <c r="H7" s="36">
         <v>38</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="36">
         <v>48</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="9" t="s">
         <v>30</v>
       </c>
@@ -4560,14 +4842,14 @@
       <c r="H8" s="36">
         <v>26</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="36">
         <v>34</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="9" t="s">
         <v>30</v>
       </c>
@@ -4592,14 +4874,14 @@
       <c r="H9" s="36">
         <v>60</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="36">
         <v>76</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="9" t="s">
         <v>30</v>
       </c>
@@ -4624,14 +4906,14 @@
       <c r="H10" s="36">
         <v>44</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="36">
         <v>50</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="9" t="s">
         <v>30</v>
       </c>
@@ -4656,14 +4938,14 @@
       <c r="H11" s="36">
         <v>24</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="36">
         <v>32</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="9" t="s">
         <v>30</v>
       </c>
@@ -4688,14 +4970,14 @@
       <c r="H12" s="36">
         <v>19</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="36">
         <v>25</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="9" t="s">
         <v>30</v>
       </c>
@@ -4720,14 +5002,14 @@
       <c r="H13" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
@@ -4752,14 +5034,14 @@
       <c r="H14" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="9" t="s">
         <v>30</v>
       </c>
@@ -4784,14 +5066,14 @@
       <c r="H15" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="37" t="s">
+      <c r="I15" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="9" t="s">
         <v>30</v>
       </c>
@@ -4810,11 +5092,11 @@
       <c r="F16" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="9" t="s">
         <v>30</v>
       </c>
@@ -4839,14 +5121,14 @@
       <c r="H17" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="9" t="s">
         <v>30</v>
       </c>
@@ -4871,14 +5153,14 @@
       <c r="H18" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="9" t="s">
         <v>30</v>
       </c>
@@ -4903,14 +5185,14 @@
       <c r="H19" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -4935,14 +5217,14 @@
       <c r="H20" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -4967,14 +5249,14 @@
       <c r="H21" s="36">
         <v>9</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="36">
         <v>19</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="9" t="s">
         <v>30</v>
       </c>
@@ -4999,14 +5281,14 @@
       <c r="H22" s="36">
         <v>76</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="36">
         <v>83</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="9" t="s">
         <v>30</v>
       </c>
@@ -5031,14 +5313,14 @@
       <c r="H23" s="36">
         <v>7</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="36">
         <v>17</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="9" t="s">
         <v>30</v>
       </c>
@@ -5057,11 +5339,11 @@
       <c r="F24" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="9" t="s">
         <v>30</v>
       </c>
@@ -5080,11 +5362,11 @@
       <c r="F25" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="9" t="s">
         <v>30</v>
       </c>
@@ -5103,8 +5385,17 @@
       <c r="F26" s="36" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="I26" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="9" t="s">
         <v>30</v>
       </c>
@@ -5123,8 +5414,11 @@
       <c r="F27" s="36" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="9" t="s">
         <v>30</v>
       </c>
@@ -5143,8 +5437,17 @@
       <c r="F28" s="36" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="I28" s="36" t="s">
+        <v>303</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="9" t="s">
         <v>30</v>
       </c>
@@ -5163,8 +5466,17 @@
       <c r="F29" s="36" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="I29" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="9" t="s">
         <v>30</v>
       </c>
@@ -5183,8 +5495,17 @@
       <c r="F30" s="36" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="36" t="s">
+        <v>306</v>
+      </c>
+      <c r="I30" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="9" t="s">
         <v>30</v>
       </c>
@@ -5203,8 +5524,11 @@
       <c r="F31" s="36" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="9" t="s">
         <v>30</v>
       </c>
@@ -5223,8 +5547,17 @@
       <c r="F32" s="36" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H32" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="I32" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="9" t="s">
         <v>30</v>
       </c>
@@ -5243,8 +5576,17 @@
       <c r="F33" s="36" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H33" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="I33" s="36" t="s">
+        <v>311</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="9" t="s">
         <v>30</v>
       </c>
@@ -5263,8 +5605,17 @@
       <c r="F34" s="36" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H34" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="I34" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="9" t="s">
         <v>30</v>
       </c>
@@ -5283,8 +5634,17 @@
       <c r="F35" s="36" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H35" s="36" t="s">
+        <v>314</v>
+      </c>
+      <c r="I35" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="9" t="s">
         <v>30</v>
       </c>
@@ -5303,8 +5663,17 @@
       <c r="F36" s="36" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H36" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="I36" s="36" t="s">
+        <v>317</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="9" t="s">
         <v>30</v>
       </c>
@@ -5323,8 +5692,17 @@
       <c r="F37" s="36" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H37" s="36" t="s">
+        <v>318</v>
+      </c>
+      <c r="I37" s="36" t="s">
+        <v>319</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="9" t="s">
         <v>30</v>
       </c>
@@ -5343,8 +5721,17 @@
       <c r="F38" s="36" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H38" s="36" t="s">
+        <v>320</v>
+      </c>
+      <c r="I38" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="9" t="s">
         <v>30</v>
       </c>
@@ -5363,8 +5750,17 @@
       <c r="F39" s="36" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H39" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="I39" s="36" t="s">
+        <v>323</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="9" t="s">
         <v>30</v>
       </c>
@@ -5383,8 +5779,17 @@
       <c r="F40" s="36" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H40" s="36" t="s">
+        <v>324</v>
+      </c>
+      <c r="I40" s="36" t="s">
+        <v>325</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="9" t="s">
         <v>30</v>
       </c>
@@ -5403,8 +5808,17 @@
       <c r="F41" s="36" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H41" s="36" t="s">
+        <v>326</v>
+      </c>
+      <c r="I41" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="9" t="s">
         <v>30</v>
       </c>
@@ -5423,8 +5837,17 @@
       <c r="F42" s="36" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H42" s="36" t="s">
+        <v>328</v>
+      </c>
+      <c r="I42" s="36" t="s">
+        <v>329</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="9" t="s">
         <v>30</v>
       </c>
@@ -5443,8 +5866,17 @@
       <c r="F43" s="36" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H43" s="36" t="s">
+        <v>330</v>
+      </c>
+      <c r="I43" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="9" t="s">
         <v>30</v>
       </c>
@@ -5463,8 +5895,17 @@
       <c r="F44" s="36" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H44" s="36" t="s">
+        <v>332</v>
+      </c>
+      <c r="I44" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="9" t="s">
         <v>30</v>
       </c>
@@ -5483,8 +5924,17 @@
       <c r="F45" s="36" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H45" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="I45" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="9" t="s">
         <v>30</v>
       </c>
@@ -5503,8 +5953,17 @@
       <c r="F46" s="36" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H46" s="36" t="s">
+        <v>326</v>
+      </c>
+      <c r="I46" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="9" t="s">
         <v>30</v>
       </c>
@@ -5523,8 +5982,17 @@
       <c r="F47" s="36" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H47" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="I47" s="36" t="s">
+        <v>336</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="9" t="s">
         <v>30</v>
       </c>
@@ -5543,8 +6011,17 @@
       <c r="F48" s="36" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H48" s="36" t="s">
+        <v>337</v>
+      </c>
+      <c r="I48" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="9" t="s">
         <v>30</v>
       </c>
@@ -5563,15 +6040,24 @@
       <c r="F49" s="36" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
+      <c r="H49" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="I49" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D50" s="35">
@@ -5583,15 +6069,24 @@
       <c r="F50" s="36" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="38" t="s">
+      <c r="H50" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="I50" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="J50" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D51" s="35">
@@ -5603,15 +6098,24 @@
       <c r="F51" s="36" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="s">
+      <c r="H51" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="I51" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="J51" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D52" s="35">
@@ -5623,15 +6127,24 @@
       <c r="F52" s="36" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="s">
+      <c r="H52" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="I52" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="J52" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D53" s="35">
@@ -5643,15 +6156,27 @@
       <c r="F53" s="36" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="s">
+      <c r="G53" s="4">
+        <v>11</v>
+      </c>
+      <c r="H53" s="36" t="s">
+        <v>254</v>
+      </c>
+      <c r="I53" s="36">
+        <v>41</v>
+      </c>
+      <c r="J53" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D54" s="35">
@@ -5663,15 +6188,24 @@
       <c r="F54" s="36" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
+      <c r="H54" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="I54" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="J54" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D55" s="35">
@@ -5683,15 +6217,27 @@
       <c r="F55" s="36" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="38" t="s">
+      <c r="G55" s="4">
+        <v>17</v>
+      </c>
+      <c r="H55" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="I55" s="36">
+        <v>61</v>
+      </c>
+      <c r="J55" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D56" s="35">
@@ -5703,15 +6249,24 @@
       <c r="F56" s="36" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="38" t="s">
+      <c r="H56" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="I56" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="J56" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D57" s="35">
@@ -5723,15 +6278,24 @@
       <c r="F57" s="36" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="38" t="s">
+      <c r="H57" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="I57" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="J57" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D58" s="35">
@@ -5743,15 +6307,24 @@
       <c r="F58" s="36" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="s">
+      <c r="H58" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="I58" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="J58" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="38" t="s">
         <v>72</v>
       </c>
       <c r="D59" s="35">
@@ -5763,15 +6336,24 @@
       <c r="F59" s="36" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="H59" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="I59" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="J59" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D60" s="35">
@@ -5783,15 +6365,24 @@
       <c r="F60" s="36" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="H60" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="I60" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="J60" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D61" s="35">
@@ -5803,15 +6394,24 @@
       <c r="F61" s="36" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="H61" s="36" t="s">
+        <v>269</v>
+      </c>
+      <c r="I61" s="36">
+        <v>42</v>
+      </c>
+      <c r="J61" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D62" s="35">
@@ -5823,15 +6423,24 @@
       <c r="F62" s="36" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="H62" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="I62" s="36">
+        <v>78</v>
+      </c>
+      <c r="J62" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D63" s="35">
@@ -5843,15 +6452,24 @@
       <c r="F63" s="36" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="H63" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="I63" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="J63" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D64" s="35">
@@ -5863,15 +6481,24 @@
       <c r="F64" s="36" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="H64" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="I64" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="J64" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D65" s="35">
@@ -5883,15 +6510,24 @@
       <c r="F65" s="36" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="H65" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="I65" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="J65" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D66" s="35">
@@ -5903,15 +6539,24 @@
       <c r="F66" s="36" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="H66" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="I66" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="J66" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D67" s="35">
@@ -5923,15 +6568,24 @@
       <c r="F67" s="36" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="H67" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="I67" s="36" t="s">
+        <v>279</v>
+      </c>
+      <c r="J67" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D68" s="35">
@@ -5943,15 +6597,24 @@
       <c r="F68" s="36" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="H68" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="I68" s="36">
+        <v>32</v>
+      </c>
+      <c r="J68" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D69" s="35">
@@ -5963,15 +6626,24 @@
       <c r="F69" s="36" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="H69" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="I69" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="J69" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D70" s="35">
@@ -5983,15 +6655,24 @@
       <c r="F70" s="36" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="H70" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="I70" s="36">
+        <v>75</v>
+      </c>
+      <c r="J70" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D71" s="35">
@@ -6003,15 +6684,24 @@
       <c r="F71" s="36" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="H71" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="I71" s="36" t="s">
+        <v>286</v>
+      </c>
+      <c r="J71" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D72" s="35">
@@ -6023,15 +6713,24 @@
       <c r="F72" s="36" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="H72" s="36" t="s">
+        <v>288</v>
+      </c>
+      <c r="I72" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="J72" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="38" t="s">
         <v>235</v>
       </c>
       <c r="D73" s="35">
@@ -6043,15 +6742,18 @@
       <c r="F73" s="36" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="J73" s="36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="38" t="s">
         <v>235</v>
       </c>
       <c r="D74" s="35">
@@ -6063,35 +6765,48 @@
       <c r="F74" s="36" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="J74" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" s="39" customFormat="1" ht="130.5" customHeight="1">
+      <c r="A75" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="D75" s="35">
+      <c r="D75" s="42">
         <v>1</v>
       </c>
-      <c r="E75" s="36" t="s">
+      <c r="E75" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="F75" s="36" t="s">
+      <c r="F75" s="40" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="G75" s="43"/>
+      <c r="H75" s="44" t="s">
+        <v>290</v>
+      </c>
+      <c r="I75" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="J75" s="40" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="38" t="s">
         <v>77</v>
       </c>
       <c r="D76" s="35">
@@ -6103,15 +6818,24 @@
       <c r="F76" s="36" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="H76" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="I76" s="36" t="s">
+        <v>292</v>
+      </c>
+      <c r="J76" s="40" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="38" t="s">
         <v>77</v>
       </c>
       <c r="D77" s="35">
@@ -6123,48 +6847,76 @@
       <c r="F77" s="36" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="H77" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="I77" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="J77" s="40" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" s="43" customFormat="1" ht="60">
+      <c r="A78" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D78" s="35">
+      <c r="D78" s="42">
         <v>4</v>
       </c>
-      <c r="E78" s="36" t="s">
+      <c r="E78" s="40" t="s">
         <v>245</v>
       </c>
-      <c r="F78" s="36" t="s">
+      <c r="F78" s="40" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="H78" s="44" t="s">
+        <v>299</v>
+      </c>
+      <c r="I78" s="44" t="s">
+        <v>297</v>
+      </c>
+      <c r="J78" s="40" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" s="39" customFormat="1" ht="45">
+      <c r="A79" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="D79" s="35">
+      <c r="D79" s="42">
         <v>5</v>
       </c>
-      <c r="E79" s="36" t="s">
+      <c r="E79" s="40" t="s">
         <v>247</v>
       </c>
-      <c r="F79" s="36" t="s">
+      <c r="F79" s="40" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" s="43"/>
+      <c r="H79" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="I79" s="44" t="s">
+        <v>296</v>
+      </c>
+      <c r="J79" s="40" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="D80" s="35"/>
     </row>
   </sheetData>

</xml_diff>